<commit_message>
minor spelling errors corrected
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
@@ -460,9 +460,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="662">
+  <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1197,7 +1199,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="662">
+  <cellStyles count="664">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1528,6 +1530,7 @@
     <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="659" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1858,6 +1861,7 @@
     <cellStyle name="Hyperlink" xfId="656" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="658" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="660" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="662" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2196,8 +2200,8 @@
   <dimension ref="A1:H367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
preparing to add elements required for dashboard
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="26840" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>Person Race</t>
   </si>
   <si>
-    <t>Preson Sex</t>
-  </si>
-  <si>
     <t>The amount of the bond</t>
   </si>
   <si>
@@ -343,13 +340,45 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCellIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <r>
+      <t>Pe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>son Sex</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -462,669 +491,669 @@
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1134,47 +1163,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1186,9 +1215,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1197,6 +1223,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="664">
@@ -2200,8 +2229,8 @@
   <dimension ref="A1:H367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2218,10 +2247,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="21"/>
+      <c r="A1" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="24"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2272,7 +2301,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>10</v>
@@ -2293,7 +2322,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>10</v>
@@ -2307,7 +2336,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2325,7 +2354,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -2346,7 +2375,7 @@
         <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -2360,7 +2389,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2378,7 +2407,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>23</v>
@@ -2399,7 +2428,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -2416,7 +2445,7 @@
         <v>38</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
@@ -2430,13 +2459,13 @@
     <row r="13" spans="1:8" ht="45">
       <c r="A13" s="10"/>
       <c r="B13" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>78</v>
-      </c>
       <c r="D13" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -2448,13 +2477,13 @@
     <row r="14" spans="1:8" ht="45">
       <c r="A14" s="10"/>
       <c r="B14" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="19" t="s">
@@ -2466,13 +2495,13 @@
     <row r="15" spans="1:8" ht="45">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>23</v>
@@ -2488,13 +2517,13 @@
     <row r="16" spans="1:8" ht="45">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>23</v>
@@ -2510,13 +2539,13 @@
     <row r="17" spans="1:8" ht="45">
       <c r="A17" s="10"/>
       <c r="B17" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>23</v>
@@ -2534,11 +2563,11 @@
       <c r="B18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>39</v>
+      <c r="C18" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>23</v>
@@ -2566,10 +2595,10 @@
         <v>20</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>23</v>
@@ -2583,10 +2612,10 @@
         <v>21</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>23</v>
@@ -2607,21 +2636,21 @@
     </row>
     <row r="23" spans="1:8" s="15" customFormat="1" ht="30">
       <c r="B23" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="22" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2634,7 +2663,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>23</v>
@@ -2649,11 +2678,11 @@
       <c r="B25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>51</v>
+      <c r="C25" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9" t="s">
@@ -2663,7 +2692,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -2678,10 +2707,10 @@
         <v>22</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>23</v>
@@ -2691,7 +2720,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -2706,10 +2735,10 @@
         <v>19</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>23</v>
@@ -2723,10 +2752,10 @@
         <v>9</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>23</v>
@@ -2740,10 +2769,10 @@
         <v>18</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>23</v>
@@ -2753,7 +2782,7 @@
     </row>
     <row r="32" spans="1:8" ht="30">
       <c r="A32" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -2768,10 +2797,10 @@
         <v>26</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="14" t="s">
@@ -2788,10 +2817,10 @@
         <v>25</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="14" t="s">
@@ -2802,16 +2831,16 @@
     </row>
     <row r="35" spans="1:8" ht="45">
       <c r="A35" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>23</v>
@@ -2822,16 +2851,16 @@
     </row>
     <row r="36" spans="1:8" ht="45">
       <c r="A36" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>23</v>
@@ -2842,13 +2871,13 @@
     </row>
     <row r="37" spans="1:8" ht="45">
       <c r="B37" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>23</v>
@@ -2862,16 +2891,16 @@
     <row r="38" spans="1:8" ht="45">
       <c r="A38" s="14"/>
       <c r="B38" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E38" s="14"/>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="21" t="s">
         <v>23</v>
       </c>
       <c r="G38" s="14"/>
@@ -2880,16 +2909,16 @@
     <row r="39" spans="1:8" ht="45">
       <c r="A39" s="14"/>
       <c r="B39" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E39" s="14"/>
-      <c r="F39" s="22" t="s">
+      <c r="F39" s="21" t="s">
         <v>23</v>
       </c>
       <c r="G39" s="14"/>
@@ -2898,16 +2927,16 @@
     <row r="40" spans="1:8" ht="45">
       <c r="A40" s="14"/>
       <c r="B40" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E40" s="14"/>
-      <c r="F40" s="22" t="s">
+      <c r="F40" s="21" t="s">
         <v>23</v>
       </c>
       <c r="G40" s="14"/>
@@ -6190,7 +6219,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
modifications to IEPD based on discussions with AO & JD
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
@@ -312,15 +312,6 @@
     <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonEthnicityText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonRaceText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonStateIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
   </si>
   <si>
@@ -328,9 +319,6 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonSexText</t>
   </si>
   <si>
     <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionAreaIdentification/nc:IdentificationID</t>
@@ -366,19 +354,24 @@
       <t>son Sex</t>
     </r>
   </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonEthnicityCode</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -491,669 +484,669 @@
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1163,47 +1156,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1224,7 +1217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2228,9 +2221,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H367"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2428,7 +2421,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -2445,7 +2438,7 @@
         <v>38</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
@@ -2483,7 +2476,7 @@
         <v>78</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="19" t="s">
@@ -2501,7 +2494,7 @@
         <v>80</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>23</v>
@@ -2523,7 +2516,7 @@
         <v>81</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>23</v>
@@ -2545,7 +2538,7 @@
         <v>82</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>23</v>
@@ -2564,10 +2557,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>23</v>
@@ -2897,7 +2890,7 @@
         <v>92</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="21" t="s">
@@ -2915,7 +2908,7 @@
         <v>93</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="21" t="s">
@@ -2933,7 +2926,7 @@
         <v>94</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="21" t="s">
@@ -6219,7 +6212,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
added elements for pretrial status and bed type
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26840" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="540" yWindow="160" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="114">
   <si>
     <t>Race</t>
   </si>
@@ -365,6 +365,24 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Bed Type</t>
+  </si>
+  <si>
+    <t>a code to describe the type of bed used by the subject</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:BedCategoryCode</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:PreTrialCategoryCode</t>
+  </si>
+  <si>
+    <t>PreTrial Status</t>
+  </si>
+  <si>
+    <t>a code to describe the status of the subject prior to trial</t>
   </si>
 </sst>
 </file>
@@ -482,9 +500,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="664">
+  <cellStyleXfs count="670">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1221,7 +1245,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="664">
+  <cellStyles count="670">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1553,6 +1577,9 @@
     <cellStyle name="Followed Hyperlink" xfId="659" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="669" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1884,6 +1911,9 @@
     <cellStyle name="Hyperlink" xfId="658" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="660" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="662" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="664" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="666" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="668" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2221,9 +2251,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H367"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2935,21 +2965,33 @@
       <c r="G40" s="14"/>
       <c r="H40" s="14"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" ht="30">
       <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
+      <c r="B41" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" ht="30">
       <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
+      <c r="B42" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>111</v>
+      </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>

</xml_diff>

<commit_message>
corrections to booking reporting mapping
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
@@ -373,9 +373,6 @@
     <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:PreTrialCategoryCode</t>
   </si>
   <si>
-    <t>PreTrial Status</t>
-  </si>
-  <si>
     <t>a code to describe the status of the subject prior to trial</t>
   </si>
   <si>
@@ -429,19 +426,15 @@
   <si>
     <t>we have this as PreTrialCategoryCode under Detention class</t>
   </si>
+  <si>
+    <t>PreTrial Status (Case Status)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -554,683 +547,683 @@
   </borders>
   <cellStyleXfs count="678">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1240,47 +1233,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1301,11 +1294,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="678">
@@ -2323,8 +2316,8 @@
   <dimension ref="A1:H370"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2341,10 +2334,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2706,7 +2699,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>61</v>
@@ -2722,13 +2715,13 @@
         <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="24" t="s">
         <v>119</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>120</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -2895,13 +2888,13 @@
         <v>48</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="14"/>
@@ -2912,13 +2905,13 @@
         <v>48</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -2980,7 +2973,7 @@
         <v>16</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>72</v>
@@ -3107,11 +3100,11 @@
       <c r="A45" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="D45" s="18" t="s">
         <v>109</v>
@@ -6378,7 +6371,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Updated Booking Reporting and Custody Query Results IEPDs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/BookingReportMapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15045" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -2643,27 +2643,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.375" style="4" customWidth="1"/>
     <col min="2" max="2" width="21" style="4" customWidth="1"/>
-    <col min="3" max="4" width="28.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="92.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="4" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="31.6640625" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="4"/>
+    <col min="3" max="4" width="28.375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="92.375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.625" style="4" customWidth="1"/>
+    <col min="10" max="11" width="10.875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="31.625" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>50</v>
       </c>
@@ -2675,7 +2675,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="45">
+    <row r="2" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
@@ -2729,7 +2729,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="30">
+    <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>7</v>
@@ -2751,7 +2751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="10" t="s">
         <v>5</v>
@@ -2773,7 +2773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>52</v>
       </c>
@@ -2789,7 +2789,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" t="s">
         <v>29</v>
@@ -2811,7 +2811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8" t="s">
         <v>30</v>
@@ -2833,7 +2833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>51</v>
       </c>
@@ -2849,7 +2849,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" ht="30">
+    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
         <v>14</v>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="K10" s="24"/>
     </row>
-    <row r="11" spans="1:12" ht="30">
+    <row r="11" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>2</v>
@@ -2903,7 +2903,7 @@
       </c>
       <c r="K11" s="24"/>
     </row>
-    <row r="12" spans="1:12" ht="30">
+    <row r="12" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9" t="s">
         <v>0</v>
@@ -2930,7 +2930,7 @@
       </c>
       <c r="K12" s="24"/>
     </row>
-    <row r="13" spans="1:12" ht="45">
+    <row r="13" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
         <v>54</v>
@@ -2960,7 +2960,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="45">
+    <row r="14" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
         <v>57</v>
@@ -2990,7 +2990,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45">
+    <row r="15" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
         <v>61</v>
@@ -3022,7 +3022,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="45">
+    <row r="16" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9" t="s">
         <v>62</v>
@@ -3054,7 +3054,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="45">
+    <row r="17" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
         <v>63</v>
@@ -3086,7 +3086,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="30">
+    <row r="18" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9" t="s">
         <v>1</v>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="K18" s="24"/>
     </row>
-    <row r="19" spans="1:12" ht="30">
+    <row r="19" spans="1:12" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="10" t="s">
         <v>122</v>
@@ -3137,7 +3137,7 @@
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
     </row>
-    <row r="20" spans="1:12" ht="45">
+    <row r="20" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>44</v>
       </c>
@@ -3163,7 +3163,7 @@
       <c r="K20" s="33"/>
       <c r="L20" s="33"/>
     </row>
-    <row r="21" spans="1:12" ht="45">
+    <row r="21" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10" t="s">
         <v>103</v>
@@ -3187,7 +3187,7 @@
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
     </row>
-    <row r="22" spans="1:12" ht="45">
+    <row r="22" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10" t="s">
         <v>104</v>
@@ -3211,7 +3211,7 @@
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
     </row>
-    <row r="23" spans="1:12" ht="45">
+    <row r="23" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="28" t="s">
         <v>105</v>
@@ -3235,7 +3235,7 @@
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
     </row>
-    <row r="24" spans="1:12" ht="30">
+    <row r="24" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10" t="s">
         <v>102</v>
@@ -3259,7 +3259,7 @@
       <c r="K24" s="33"/>
       <c r="L24" s="33"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -3275,7 +3275,7 @@
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
     </row>
-    <row r="26" spans="1:12" ht="30">
+    <row r="26" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="10" t="s">
         <v>18</v>
@@ -3298,7 +3298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="30">
+    <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="10" t="s">
         <v>19</v>
@@ -3322,7 +3322,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="75">
+    <row r="28" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
       <c r="B28" s="35" t="s">
         <v>79</v>
@@ -3348,7 +3348,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -3364,7 +3364,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
     </row>
-    <row r="30" spans="1:12" s="14" customFormat="1" ht="30">
+    <row r="30" spans="1:12" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
         <v>53</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30">
+    <row r="31" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="9" t="s">
         <v>161</v>
@@ -3417,7 +3417,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="45">
+    <row r="32" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="9" t="s">
         <v>22</v>
@@ -3439,7 +3439,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>43</v>
       </c>
@@ -3455,7 +3455,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
     </row>
-    <row r="34" spans="1:12" ht="30">
+    <row r="34" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="37" t="s">
         <v>110</v>
@@ -3479,7 +3479,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="31.5" customHeight="1">
+    <row r="35" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="10" t="s">
         <v>20</v>
@@ -3502,7 +3502,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>40</v>
       </c>
@@ -3518,7 +3518,7 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
     </row>
-    <row r="37" spans="1:12" ht="30">
+    <row r="37" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="10" t="s">
         <v>17</v>
@@ -3541,7 +3541,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="30">
+    <row r="38" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="10" t="s">
         <v>9</v>
@@ -3564,7 +3564,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="45">
+    <row r="39" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="10" t="s">
         <v>109</v>
@@ -3587,7 +3587,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="165">
+    <row r="40" spans="1:12" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A40" s="34"/>
       <c r="B40" s="35" t="s">
         <v>89</v>
@@ -3613,7 +3613,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="30">
+    <row r="41" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>44</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>164</v>
       </c>
@@ -3652,7 +3652,7 @@
       <c r="K42" s="7"/>
       <c r="L42" s="26"/>
     </row>
-    <row r="43" spans="1:12" ht="60">
+    <row r="43" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A43" s="34"/>
       <c r="B43" s="39" t="s">
         <v>163</v>
@@ -3676,7 +3676,7 @@
       <c r="K43" s="33"/>
       <c r="L43" s="33"/>
     </row>
-    <row r="44" spans="1:12" ht="60">
+    <row r="44" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A44" s="36"/>
       <c r="B44" s="38" t="s">
         <v>88</v>
@@ -3696,7 +3696,7 @@
       <c r="K44" s="33"/>
       <c r="L44" s="33"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>98</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="K45" s="7"/>
       <c r="L45" s="26"/>
     </row>
-    <row r="46" spans="1:12" ht="45">
+    <row r="46" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="10" t="s">
         <v>166</v>
@@ -3737,7 +3737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="30">
+    <row r="47" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="10" t="s">
         <v>23</v>
@@ -3763,7 +3763,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="45">
+    <row r="48" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>44</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="45">
+    <row r="49" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>44</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="45">
+    <row r="50" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
         <v>42</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="45">
+    <row r="51" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="9" t="s">
         <v>64</v>
@@ -3866,7 +3866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="45">
+    <row r="52" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="9" t="s">
         <v>65</v>
@@ -3888,7 +3888,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="45">
+    <row r="53" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="4" t="s">
         <v>66</v>
@@ -3910,7 +3910,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="45">
+    <row r="54" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>171</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="30">
+    <row r="55" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>171</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="30">
+    <row r="56" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A56" s="34"/>
       <c r="B56" s="38" t="s">
         <v>92</v>
@@ -3982,7 +3982,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="30">
+    <row r="57" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="s">
         <v>44</v>
       </c>
@@ -4008,7 +4008,7 @@
       <c r="K57" s="33"/>
       <c r="L57" s="33"/>
     </row>
-    <row r="58" spans="1:12" ht="30">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="34" t="s">
         <v>44</v>
       </c>
@@ -4034,7 +4034,7 @@
       <c r="K58" s="33"/>
       <c r="L58" s="33"/>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="20"/>
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
@@ -4045,7 +4045,7 @@
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="E60" s="13"/>
@@ -4054,7 +4054,7 @@
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
         <v>85</v>
       </c>
@@ -4065,7 +4065,7 @@
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:12" ht="60">
+    <row r="62" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A62" s="20"/>
       <c r="B62" s="20" t="s">
         <v>86</v>
@@ -4080,7 +4080,7 @@
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="E63" s="13"/>
@@ -4089,7 +4089,7 @@
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="E64" s="13"/>
@@ -4098,7 +4098,7 @@
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="E65" s="13"/>
@@ -4107,7 +4107,7 @@
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="E66" s="13"/>
@@ -4116,7 +4116,7 @@
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="E67" s="13"/>
@@ -4125,7 +4125,7 @@
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="E68" s="13"/>
@@ -4134,7 +4134,7 @@
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="E69" s="13"/>
@@ -4143,7 +4143,7 @@
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="E70" s="13"/>
@@ -4152,7 +4152,7 @@
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="E71" s="13"/>
@@ -4161,7 +4161,7 @@
       <c r="H71" s="13"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="E72" s="13"/>
@@ -4170,7 +4170,7 @@
       <c r="H72" s="13"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="E73" s="13"/>
@@ -4179,7 +4179,7 @@
       <c r="H73" s="13"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="E74" s="13"/>
@@ -4188,7 +4188,7 @@
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="E75" s="13"/>
@@ -4197,7 +4197,7 @@
       <c r="H75" s="13"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="E76" s="13"/>
@@ -4206,7 +4206,7 @@
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="E77" s="13"/>
@@ -4215,7 +4215,7 @@
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="E78" s="13"/>
@@ -4224,7 +4224,7 @@
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="E79" s="13"/>
@@ -4233,7 +4233,7 @@
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="E80" s="13"/>
@@ -4242,7 +4242,7 @@
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="E81" s="13"/>
@@ -4251,7 +4251,7 @@
       <c r="H81" s="13"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="E82" s="13"/>
@@ -4260,7 +4260,7 @@
       <c r="H82" s="13"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="E83" s="13"/>
@@ -4269,7 +4269,7 @@
       <c r="H83" s="13"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="E84" s="13"/>
@@ -4278,7 +4278,7 @@
       <c r="H84" s="13"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="E85" s="13"/>
@@ -4287,7 +4287,7 @@
       <c r="H85" s="13"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="E86" s="13"/>
@@ -4296,7 +4296,7 @@
       <c r="H86" s="13"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="E87" s="13"/>
@@ -4305,7 +4305,7 @@
       <c r="H87" s="13"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="E88" s="13"/>
@@ -4314,7 +4314,7 @@
       <c r="H88" s="13"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="E89" s="13"/>
@@ -4323,7 +4323,7 @@
       <c r="H89" s="13"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="E90" s="13"/>
@@ -4332,7 +4332,7 @@
       <c r="H90" s="13"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="E91" s="13"/>
@@ -4341,7 +4341,7 @@
       <c r="H91" s="13"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="E92" s="13"/>
@@ -4350,7 +4350,7 @@
       <c r="H92" s="13"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="E93" s="13"/>
@@ -4359,7 +4359,7 @@
       <c r="H93" s="13"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="E94" s="13"/>
@@ -4368,7 +4368,7 @@
       <c r="H94" s="13"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="E95" s="13"/>
@@ -4377,7 +4377,7 @@
       <c r="H95" s="13"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="E96" s="13"/>
@@ -4386,7 +4386,7 @@
       <c r="H96" s="13"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="E97" s="13"/>
@@ -4395,7 +4395,7 @@
       <c r="H97" s="13"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="E98" s="13"/>
@@ -4404,7 +4404,7 @@
       <c r="H98" s="13"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="E99" s="13"/>
@@ -4413,7 +4413,7 @@
       <c r="H99" s="13"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="E100" s="13"/>
@@ -4422,7 +4422,7 @@
       <c r="H100" s="13"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="E101" s="13"/>
@@ -4431,7 +4431,7 @@
       <c r="H101" s="13"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="13"/>
       <c r="B102" s="13"/>
       <c r="E102" s="13"/>
@@ -4440,7 +4440,7 @@
       <c r="H102" s="13"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="13"/>
       <c r="B103" s="13"/>
       <c r="E103" s="13"/>
@@ -4449,7 +4449,7 @@
       <c r="H103" s="13"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="13"/>
       <c r="B104" s="13"/>
       <c r="E104" s="13"/>
@@ -4458,7 +4458,7 @@
       <c r="H104" s="13"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="13"/>
       <c r="B105" s="13"/>
       <c r="E105" s="13"/>
@@ -4467,7 +4467,7 @@
       <c r="H105" s="13"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="E106" s="13"/>
@@ -4476,7 +4476,7 @@
       <c r="H106" s="13"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
       <c r="B107" s="13"/>
       <c r="E107" s="13"/>
@@ -4485,7 +4485,7 @@
       <c r="H107" s="13"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
       <c r="E108" s="13"/>
@@ -4494,7 +4494,7 @@
       <c r="H108" s="13"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="13"/>
       <c r="B109" s="13"/>
       <c r="E109" s="13"/>
@@ -4503,7 +4503,7 @@
       <c r="H109" s="13"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
       <c r="E110" s="13"/>
@@ -4512,7 +4512,7 @@
       <c r="H110" s="13"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="13"/>
       <c r="B111" s="13"/>
       <c r="E111" s="13"/>
@@ -4521,7 +4521,7 @@
       <c r="H111" s="13"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="E112" s="13"/>
@@ -4530,7 +4530,7 @@
       <c r="H112" s="13"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="13"/>
       <c r="B113" s="13"/>
       <c r="E113" s="13"/>
@@ -4539,7 +4539,7 @@
       <c r="H113" s="13"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
       <c r="B114" s="13"/>
       <c r="E114" s="13"/>
@@ -4548,7 +4548,7 @@
       <c r="H114" s="13"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="13"/>
       <c r="B115" s="13"/>
       <c r="E115" s="13"/>
@@ -4557,7 +4557,7 @@
       <c r="H115" s="13"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
       <c r="B116" s="13"/>
       <c r="E116" s="13"/>
@@ -4566,7 +4566,7 @@
       <c r="H116" s="13"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
       <c r="B117" s="13"/>
       <c r="E117" s="13"/>
@@ -4575,7 +4575,7 @@
       <c r="H117" s="13"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
       <c r="B118" s="13"/>
       <c r="E118" s="13"/>
@@ -4584,7 +4584,7 @@
       <c r="H118" s="13"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="13"/>
       <c r="B119" s="13"/>
       <c r="E119" s="13"/>
@@ -4593,7 +4593,7 @@
       <c r="H119" s="13"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="13"/>
       <c r="B120" s="13"/>
       <c r="E120" s="13"/>
@@ -4602,7 +4602,7 @@
       <c r="H120" s="13"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="13"/>
       <c r="B121" s="13"/>
       <c r="E121" s="13"/>
@@ -4611,7 +4611,7 @@
       <c r="H121" s="13"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="13"/>
       <c r="B122" s="13"/>
       <c r="E122" s="13"/>
@@ -4620,7 +4620,7 @@
       <c r="H122" s="13"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
       <c r="B123" s="13"/>
       <c r="E123" s="13"/>
@@ -4629,7 +4629,7 @@
       <c r="H123" s="13"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="13"/>
       <c r="B124" s="13"/>
       <c r="E124" s="13"/>
@@ -4638,7 +4638,7 @@
       <c r="H124" s="13"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
       <c r="B125" s="13"/>
       <c r="E125" s="13"/>
@@ -4647,7 +4647,7 @@
       <c r="H125" s="13"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
       <c r="B126" s="13"/>
       <c r="E126" s="13"/>
@@ -4656,7 +4656,7 @@
       <c r="H126" s="13"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="13"/>
       <c r="B127" s="13"/>
       <c r="E127" s="13"/>
@@ -4665,7 +4665,7 @@
       <c r="H127" s="13"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
       <c r="B128" s="13"/>
       <c r="E128" s="13"/>
@@ -4674,7 +4674,7 @@
       <c r="H128" s="13"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="13"/>
       <c r="B129" s="13"/>
       <c r="E129" s="13"/>
@@ -4683,7 +4683,7 @@
       <c r="H129" s="13"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="13"/>
       <c r="B130" s="13"/>
       <c r="E130" s="13"/>
@@ -4692,7 +4692,7 @@
       <c r="H130" s="13"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="13"/>
       <c r="B131" s="13"/>
       <c r="E131" s="13"/>
@@ -4701,7 +4701,7 @@
       <c r="H131" s="13"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="13"/>
       <c r="B132" s="13"/>
       <c r="E132" s="13"/>
@@ -4710,7 +4710,7 @@
       <c r="H132" s="13"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="13"/>
       <c r="B133" s="13"/>
       <c r="E133" s="13"/>
@@ -4719,7 +4719,7 @@
       <c r="H133" s="13"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
       <c r="B134" s="13"/>
       <c r="E134" s="13"/>
@@ -4728,7 +4728,7 @@
       <c r="H134" s="13"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="13"/>
       <c r="B135" s="13"/>
       <c r="E135" s="13"/>
@@ -4737,7 +4737,7 @@
       <c r="H135" s="13"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="13"/>
       <c r="B136" s="13"/>
       <c r="E136" s="13"/>
@@ -4746,7 +4746,7 @@
       <c r="H136" s="13"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="13"/>
       <c r="B137" s="13"/>
       <c r="E137" s="13"/>
@@ -4755,7 +4755,7 @@
       <c r="H137" s="13"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="13"/>
       <c r="B138" s="13"/>
       <c r="E138" s="13"/>
@@ -4764,7 +4764,7 @@
       <c r="H138" s="13"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="13"/>
       <c r="B139" s="13"/>
       <c r="E139" s="13"/>
@@ -4773,7 +4773,7 @@
       <c r="H139" s="13"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="13"/>
       <c r="B140" s="13"/>
       <c r="E140" s="13"/>
@@ -4782,7 +4782,7 @@
       <c r="H140" s="13"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="13"/>
       <c r="B141" s="13"/>
       <c r="E141" s="13"/>
@@ -4791,7 +4791,7 @@
       <c r="H141" s="13"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="13"/>
       <c r="B142" s="13"/>
       <c r="E142" s="13"/>
@@ -4800,7 +4800,7 @@
       <c r="H142" s="13"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="13"/>
       <c r="B143" s="13"/>
       <c r="E143" s="13"/>
@@ -4809,7 +4809,7 @@
       <c r="H143" s="13"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
       <c r="B144" s="13"/>
       <c r="E144" s="13"/>
@@ -4818,7 +4818,7 @@
       <c r="H144" s="13"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="13"/>
       <c r="B145" s="13"/>
       <c r="E145" s="13"/>
@@ -4827,7 +4827,7 @@
       <c r="H145" s="13"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="13"/>
       <c r="B146" s="13"/>
       <c r="E146" s="13"/>
@@ -4836,7 +4836,7 @@
       <c r="H146" s="13"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="13"/>
       <c r="B147" s="13"/>
       <c r="E147" s="13"/>
@@ -4845,7 +4845,7 @@
       <c r="H147" s="13"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="13"/>
       <c r="B148" s="13"/>
       <c r="E148" s="13"/>
@@ -4854,7 +4854,7 @@
       <c r="H148" s="13"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
       <c r="B149" s="13"/>
       <c r="E149" s="13"/>
@@ -4863,7 +4863,7 @@
       <c r="H149" s="13"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="13"/>
       <c r="B150" s="13"/>
       <c r="E150" s="13"/>
@@ -4872,7 +4872,7 @@
       <c r="H150" s="13"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="13"/>
       <c r="B151" s="13"/>
       <c r="E151" s="13"/>
@@ -4881,7 +4881,7 @@
       <c r="H151" s="13"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="13"/>
       <c r="B152" s="13"/>
       <c r="E152" s="13"/>
@@ -4890,7 +4890,7 @@
       <c r="H152" s="13"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="13"/>
       <c r="B153" s="13"/>
       <c r="E153" s="13"/>
@@ -4899,7 +4899,7 @@
       <c r="H153" s="13"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="13"/>
       <c r="B154" s="13"/>
       <c r="E154" s="13"/>
@@ -4908,7 +4908,7 @@
       <c r="H154" s="13"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="13"/>
       <c r="B155" s="13"/>
       <c r="E155" s="13"/>
@@ -4917,7 +4917,7 @@
       <c r="H155" s="13"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="13"/>
       <c r="B156" s="13"/>
       <c r="E156" s="13"/>
@@ -4926,7 +4926,7 @@
       <c r="H156" s="13"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
       <c r="B157" s="13"/>
       <c r="E157" s="13"/>
@@ -4935,7 +4935,7 @@
       <c r="H157" s="13"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="13"/>
       <c r="B158" s="13"/>
       <c r="E158" s="13"/>
@@ -4944,7 +4944,7 @@
       <c r="H158" s="13"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="13"/>
       <c r="B159" s="13"/>
       <c r="E159" s="13"/>
@@ -4953,7 +4953,7 @@
       <c r="H159" s="13"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="13"/>
       <c r="B160" s="13"/>
       <c r="E160" s="13"/>
@@ -4962,7 +4962,7 @@
       <c r="H160" s="13"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="13"/>
       <c r="B161" s="13"/>
       <c r="E161" s="13"/>
@@ -4971,7 +4971,7 @@
       <c r="H161" s="13"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="13"/>
       <c r="B162" s="13"/>
       <c r="E162" s="13"/>
@@ -4980,7 +4980,7 @@
       <c r="H162" s="13"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
       <c r="B163" s="13"/>
       <c r="E163" s="13"/>
@@ -4989,7 +4989,7 @@
       <c r="H163" s="13"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="13"/>
       <c r="B164" s="13"/>
       <c r="E164" s="13"/>
@@ -4998,7 +4998,7 @@
       <c r="H164" s="13"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="13"/>
       <c r="B165" s="13"/>
       <c r="E165" s="13"/>
@@ -5007,7 +5007,7 @@
       <c r="H165" s="13"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="13"/>
       <c r="B166" s="13"/>
       <c r="E166" s="13"/>
@@ -5016,7 +5016,7 @@
       <c r="H166" s="13"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="13"/>
       <c r="B167" s="13"/>
       <c r="E167" s="13"/>
@@ -5025,7 +5025,7 @@
       <c r="H167" s="13"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="13"/>
       <c r="B168" s="13"/>
       <c r="E168" s="13"/>
@@ -5034,7 +5034,7 @@
       <c r="H168" s="13"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="13"/>
       <c r="B169" s="13"/>
       <c r="E169" s="13"/>
@@ -5043,7 +5043,7 @@
       <c r="H169" s="13"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
       <c r="B170" s="13"/>
       <c r="E170" s="13"/>
@@ -5052,7 +5052,7 @@
       <c r="H170" s="13"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="13"/>
       <c r="B171" s="13"/>
       <c r="E171" s="13"/>
@@ -5061,7 +5061,7 @@
       <c r="H171" s="13"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="13"/>
       <c r="B172" s="13"/>
       <c r="E172" s="13"/>
@@ -5070,7 +5070,7 @@
       <c r="H172" s="13"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
       <c r="B173" s="13"/>
       <c r="E173" s="13"/>
@@ -5079,7 +5079,7 @@
       <c r="H173" s="13"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="13"/>
       <c r="B174" s="13"/>
       <c r="E174" s="13"/>
@@ -5088,7 +5088,7 @@
       <c r="H174" s="13"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="13"/>
       <c r="B175" s="13"/>
       <c r="E175" s="13"/>
@@ -5097,7 +5097,7 @@
       <c r="H175" s="13"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="13"/>
       <c r="B176" s="13"/>
       <c r="E176" s="13"/>
@@ -5106,7 +5106,7 @@
       <c r="H176" s="13"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="13"/>
       <c r="B177" s="13"/>
       <c r="E177" s="13"/>
@@ -5115,7 +5115,7 @@
       <c r="H177" s="13"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="13"/>
       <c r="B178" s="13"/>
       <c r="E178" s="13"/>
@@ -5124,7 +5124,7 @@
       <c r="H178" s="13"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
       <c r="B179" s="13"/>
       <c r="E179" s="13"/>
@@ -5133,7 +5133,7 @@
       <c r="H179" s="13"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="13"/>
       <c r="B180" s="13"/>
       <c r="E180" s="13"/>
@@ -5142,7 +5142,7 @@
       <c r="H180" s="13"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="13"/>
       <c r="B181" s="13"/>
       <c r="E181" s="13"/>
@@ -5151,7 +5151,7 @@
       <c r="H181" s="13"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
       <c r="B182" s="13"/>
       <c r="E182" s="13"/>
@@ -5160,7 +5160,7 @@
       <c r="H182" s="13"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="13"/>
       <c r="B183" s="13"/>
       <c r="E183" s="13"/>
@@ -5169,7 +5169,7 @@
       <c r="H183" s="13"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
       <c r="B184" s="13"/>
       <c r="E184" s="13"/>
@@ -5178,7 +5178,7 @@
       <c r="H184" s="13"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="13"/>
       <c r="B185" s="13"/>
       <c r="E185" s="13"/>
@@ -5187,7 +5187,7 @@
       <c r="H185" s="13"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="13"/>
       <c r="B186" s="13"/>
       <c r="E186" s="13"/>
@@ -5196,7 +5196,7 @@
       <c r="H186" s="13"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="13"/>
       <c r="B187" s="13"/>
       <c r="E187" s="13"/>
@@ -5205,7 +5205,7 @@
       <c r="H187" s="13"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="13"/>
       <c r="B188" s="13"/>
       <c r="E188" s="13"/>
@@ -5214,7 +5214,7 @@
       <c r="H188" s="13"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="13"/>
       <c r="B189" s="13"/>
       <c r="E189" s="13"/>
@@ -5223,7 +5223,7 @@
       <c r="H189" s="13"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="13"/>
       <c r="B190" s="13"/>
       <c r="E190" s="13"/>
@@ -5232,7 +5232,7 @@
       <c r="H190" s="13"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
       <c r="B191" s="13"/>
       <c r="E191" s="13"/>
@@ -5241,7 +5241,7 @@
       <c r="H191" s="13"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="13"/>
       <c r="B192" s="13"/>
       <c r="E192" s="13"/>
@@ -5250,7 +5250,7 @@
       <c r="H192" s="13"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="13"/>
       <c r="B193" s="13"/>
       <c r="E193" s="13"/>
@@ -5259,7 +5259,7 @@
       <c r="H193" s="13"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="13"/>
       <c r="B194" s="13"/>
       <c r="E194" s="13"/>
@@ -5268,7 +5268,7 @@
       <c r="H194" s="13"/>
       <c r="I194" s="13"/>
     </row>
-    <row r="195" spans="1:9">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="13"/>
       <c r="B195" s="13"/>
       <c r="E195" s="13"/>
@@ -5277,7 +5277,7 @@
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
     </row>
-    <row r="196" spans="1:9">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="13"/>
       <c r="B196" s="13"/>
       <c r="E196" s="13"/>
@@ -5286,7 +5286,7 @@
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="13"/>
       <c r="B197" s="13"/>
       <c r="E197" s="13"/>
@@ -5295,7 +5295,7 @@
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
     </row>
-    <row r="198" spans="1:9">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="13"/>
       <c r="B198" s="13"/>
       <c r="E198" s="13"/>
@@ -5304,7 +5304,7 @@
       <c r="H198" s="13"/>
       <c r="I198" s="13"/>
     </row>
-    <row r="199" spans="1:9">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="13"/>
       <c r="B199" s="13"/>
       <c r="E199" s="13"/>
@@ -5313,7 +5313,7 @@
       <c r="H199" s="13"/>
       <c r="I199" s="13"/>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="13"/>
       <c r="B200" s="13"/>
       <c r="E200" s="13"/>
@@ -5322,7 +5322,7 @@
       <c r="H200" s="13"/>
       <c r="I200" s="13"/>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
       <c r="B201" s="13"/>
       <c r="E201" s="13"/>
@@ -5331,7 +5331,7 @@
       <c r="H201" s="13"/>
       <c r="I201" s="13"/>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="13"/>
       <c r="B202" s="13"/>
       <c r="E202" s="13"/>
@@ -5340,7 +5340,7 @@
       <c r="H202" s="13"/>
       <c r="I202" s="13"/>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="13"/>
       <c r="B203" s="13"/>
       <c r="E203" s="13"/>
@@ -5349,7 +5349,7 @@
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="13"/>
       <c r="B204" s="13"/>
       <c r="E204" s="13"/>
@@ -5358,7 +5358,7 @@
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="13"/>
       <c r="B205" s="13"/>
       <c r="E205" s="13"/>
@@ -5367,7 +5367,7 @@
       <c r="H205" s="13"/>
       <c r="I205" s="13"/>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="13"/>
       <c r="B206" s="13"/>
       <c r="E206" s="13"/>
@@ -5376,7 +5376,7 @@
       <c r="H206" s="13"/>
       <c r="I206" s="13"/>
     </row>
-    <row r="207" spans="1:9">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
       <c r="B207" s="13"/>
       <c r="E207" s="13"/>
@@ -5385,7 +5385,7 @@
       <c r="H207" s="13"/>
       <c r="I207" s="13"/>
     </row>
-    <row r="208" spans="1:9">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="13"/>
       <c r="B208" s="13"/>
       <c r="E208" s="13"/>
@@ -5394,7 +5394,7 @@
       <c r="H208" s="13"/>
       <c r="I208" s="13"/>
     </row>
-    <row r="209" spans="1:9">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="13"/>
       <c r="B209" s="13"/>
       <c r="E209" s="13"/>
@@ -5403,7 +5403,7 @@
       <c r="H209" s="13"/>
       <c r="I209" s="13"/>
     </row>
-    <row r="210" spans="1:9">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="13"/>
       <c r="B210" s="13"/>
       <c r="E210" s="13"/>
@@ -5412,7 +5412,7 @@
       <c r="H210" s="13"/>
       <c r="I210" s="13"/>
     </row>
-    <row r="211" spans="1:9">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="13"/>
       <c r="B211" s="13"/>
       <c r="E211" s="13"/>
@@ -5421,7 +5421,7 @@
       <c r="H211" s="13"/>
       <c r="I211" s="13"/>
     </row>
-    <row r="212" spans="1:9">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="13"/>
       <c r="B212" s="13"/>
       <c r="E212" s="13"/>
@@ -5430,7 +5430,7 @@
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
     </row>
-    <row r="213" spans="1:9">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="13"/>
       <c r="B213" s="13"/>
       <c r="E213" s="13"/>
@@ -5439,7 +5439,7 @@
       <c r="H213" s="13"/>
       <c r="I213" s="13"/>
     </row>
-    <row r="214" spans="1:9">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="13"/>
       <c r="B214" s="13"/>
       <c r="E214" s="13"/>
@@ -5448,7 +5448,7 @@
       <c r="H214" s="13"/>
       <c r="I214" s="13"/>
     </row>
-    <row r="215" spans="1:9">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
       <c r="B215" s="13"/>
       <c r="E215" s="13"/>
@@ -5457,7 +5457,7 @@
       <c r="H215" s="13"/>
       <c r="I215" s="13"/>
     </row>
-    <row r="216" spans="1:9">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="13"/>
       <c r="B216" s="13"/>
       <c r="E216" s="13"/>
@@ -5466,7 +5466,7 @@
       <c r="H216" s="13"/>
       <c r="I216" s="13"/>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="13"/>
       <c r="B217" s="13"/>
       <c r="E217" s="13"/>
@@ -5475,7 +5475,7 @@
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
     </row>
-    <row r="218" spans="1:9">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="13"/>
       <c r="B218" s="13"/>
       <c r="E218" s="13"/>
@@ -5484,7 +5484,7 @@
       <c r="H218" s="13"/>
       <c r="I218" s="13"/>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="13"/>
       <c r="B219" s="13"/>
       <c r="E219" s="13"/>
@@ -5493,7 +5493,7 @@
       <c r="H219" s="13"/>
       <c r="I219" s="13"/>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="13"/>
       <c r="B220" s="13"/>
       <c r="E220" s="13"/>
@@ -5502,7 +5502,7 @@
       <c r="H220" s="13"/>
       <c r="I220" s="13"/>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="13"/>
       <c r="B221" s="13"/>
       <c r="E221" s="13"/>
@@ -5511,7 +5511,7 @@
       <c r="H221" s="13"/>
       <c r="I221" s="13"/>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="13"/>
       <c r="B222" s="13"/>
       <c r="E222" s="13"/>
@@ -5520,7 +5520,7 @@
       <c r="H222" s="13"/>
       <c r="I222" s="13"/>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="13"/>
       <c r="B223" s="13"/>
       <c r="E223" s="13"/>
@@ -5529,7 +5529,7 @@
       <c r="H223" s="13"/>
       <c r="I223" s="13"/>
     </row>
-    <row r="224" spans="1:9">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="13"/>
       <c r="B224" s="13"/>
       <c r="E224" s="13"/>
@@ -5538,7 +5538,7 @@
       <c r="H224" s="13"/>
       <c r="I224" s="13"/>
     </row>
-    <row r="225" spans="1:9">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="13"/>
       <c r="B225" s="13"/>
       <c r="E225" s="13"/>
@@ -5547,7 +5547,7 @@
       <c r="H225" s="13"/>
       <c r="I225" s="13"/>
     </row>
-    <row r="226" spans="1:9">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="13"/>
       <c r="B226" s="13"/>
       <c r="E226" s="13"/>
@@ -5556,7 +5556,7 @@
       <c r="H226" s="13"/>
       <c r="I226" s="13"/>
     </row>
-    <row r="227" spans="1:9">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="13"/>
       <c r="B227" s="13"/>
       <c r="E227" s="13"/>
@@ -5565,7 +5565,7 @@
       <c r="H227" s="13"/>
       <c r="I227" s="13"/>
     </row>
-    <row r="228" spans="1:9">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="13"/>
       <c r="B228" s="13"/>
       <c r="E228" s="13"/>
@@ -5574,7 +5574,7 @@
       <c r="H228" s="13"/>
       <c r="I228" s="13"/>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="13"/>
       <c r="B229" s="13"/>
       <c r="E229" s="13"/>
@@ -5583,7 +5583,7 @@
       <c r="H229" s="13"/>
       <c r="I229" s="13"/>
     </row>
-    <row r="230" spans="1:9">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="13"/>
       <c r="B230" s="13"/>
       <c r="E230" s="13"/>
@@ -5592,7 +5592,7 @@
       <c r="H230" s="13"/>
       <c r="I230" s="13"/>
     </row>
-    <row r="231" spans="1:9">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="13"/>
       <c r="B231" s="13"/>
       <c r="E231" s="13"/>
@@ -5601,7 +5601,7 @@
       <c r="H231" s="13"/>
       <c r="I231" s="13"/>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="13"/>
       <c r="B232" s="13"/>
       <c r="E232" s="13"/>
@@ -5610,7 +5610,7 @@
       <c r="H232" s="13"/>
       <c r="I232" s="13"/>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="13"/>
       <c r="B233" s="13"/>
       <c r="E233" s="13"/>
@@ -5619,7 +5619,7 @@
       <c r="H233" s="13"/>
       <c r="I233" s="13"/>
     </row>
-    <row r="234" spans="1:9">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="13"/>
       <c r="B234" s="13"/>
       <c r="E234" s="13"/>
@@ -5628,7 +5628,7 @@
       <c r="H234" s="13"/>
       <c r="I234" s="13"/>
     </row>
-    <row r="235" spans="1:9">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="13"/>
       <c r="B235" s="13"/>
       <c r="E235" s="13"/>
@@ -5637,7 +5637,7 @@
       <c r="H235" s="13"/>
       <c r="I235" s="13"/>
     </row>
-    <row r="236" spans="1:9">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="13"/>
       <c r="B236" s="13"/>
       <c r="E236" s="13"/>
@@ -5646,7 +5646,7 @@
       <c r="H236" s="13"/>
       <c r="I236" s="13"/>
     </row>
-    <row r="237" spans="1:9">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="13"/>
       <c r="B237" s="13"/>
       <c r="E237" s="13"/>
@@ -5655,7 +5655,7 @@
       <c r="H237" s="13"/>
       <c r="I237" s="13"/>
     </row>
-    <row r="238" spans="1:9">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="13"/>
       <c r="B238" s="13"/>
       <c r="E238" s="13"/>
@@ -5664,7 +5664,7 @@
       <c r="H238" s="13"/>
       <c r="I238" s="13"/>
     </row>
-    <row r="239" spans="1:9">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="13"/>
       <c r="B239" s="13"/>
       <c r="E239" s="13"/>
@@ -5673,7 +5673,7 @@
       <c r="H239" s="13"/>
       <c r="I239" s="13"/>
     </row>
-    <row r="240" spans="1:9">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="13"/>
       <c r="B240" s="13"/>
       <c r="E240" s="13"/>
@@ -5682,7 +5682,7 @@
       <c r="H240" s="13"/>
       <c r="I240" s="13"/>
     </row>
-    <row r="241" spans="1:9">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="13"/>
       <c r="B241" s="13"/>
       <c r="E241" s="13"/>
@@ -5691,7 +5691,7 @@
       <c r="H241" s="13"/>
       <c r="I241" s="13"/>
     </row>
-    <row r="242" spans="1:9">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="13"/>
       <c r="B242" s="13"/>
       <c r="E242" s="13"/>
@@ -5700,7 +5700,7 @@
       <c r="H242" s="13"/>
       <c r="I242" s="13"/>
     </row>
-    <row r="243" spans="1:9">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="13"/>
       <c r="B243" s="13"/>
       <c r="E243" s="13"/>
@@ -5709,7 +5709,7 @@
       <c r="H243" s="13"/>
       <c r="I243" s="13"/>
     </row>
-    <row r="244" spans="1:9">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="13"/>
       <c r="B244" s="13"/>
       <c r="E244" s="13"/>
@@ -5718,7 +5718,7 @@
       <c r="H244" s="13"/>
       <c r="I244" s="13"/>
     </row>
-    <row r="245" spans="1:9">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="13"/>
       <c r="B245" s="13"/>
       <c r="E245" s="13"/>
@@ -5727,7 +5727,7 @@
       <c r="H245" s="13"/>
       <c r="I245" s="13"/>
     </row>
-    <row r="246" spans="1:9">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="13"/>
       <c r="B246" s="13"/>
       <c r="E246" s="13"/>
@@ -5736,7 +5736,7 @@
       <c r="H246" s="13"/>
       <c r="I246" s="13"/>
     </row>
-    <row r="247" spans="1:9">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="13"/>
       <c r="B247" s="13"/>
       <c r="E247" s="13"/>
@@ -5745,7 +5745,7 @@
       <c r="H247" s="13"/>
       <c r="I247" s="13"/>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="13"/>
       <c r="B248" s="13"/>
       <c r="E248" s="13"/>
@@ -5754,7 +5754,7 @@
       <c r="H248" s="13"/>
       <c r="I248" s="13"/>
     </row>
-    <row r="249" spans="1:9">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="13"/>
       <c r="B249" s="13"/>
       <c r="E249" s="13"/>
@@ -5763,7 +5763,7 @@
       <c r="H249" s="13"/>
       <c r="I249" s="13"/>
     </row>
-    <row r="250" spans="1:9">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="13"/>
       <c r="B250" s="13"/>
       <c r="E250" s="13"/>
@@ -5772,7 +5772,7 @@
       <c r="H250" s="13"/>
       <c r="I250" s="13"/>
     </row>
-    <row r="251" spans="1:9">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="13"/>
       <c r="B251" s="13"/>
       <c r="E251" s="13"/>
@@ -5781,7 +5781,7 @@
       <c r="H251" s="13"/>
       <c r="I251" s="13"/>
     </row>
-    <row r="252" spans="1:9">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" s="13"/>
       <c r="B252" s="13"/>
       <c r="E252" s="13"/>
@@ -5790,7 +5790,7 @@
       <c r="H252" s="13"/>
       <c r="I252" s="13"/>
     </row>
-    <row r="253" spans="1:9">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="13"/>
       <c r="B253" s="13"/>
       <c r="E253" s="13"/>
@@ -5799,7 +5799,7 @@
       <c r="H253" s="13"/>
       <c r="I253" s="13"/>
     </row>
-    <row r="254" spans="1:9">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="13"/>
       <c r="B254" s="13"/>
       <c r="E254" s="13"/>
@@ -5808,7 +5808,7 @@
       <c r="H254" s="13"/>
       <c r="I254" s="13"/>
     </row>
-    <row r="255" spans="1:9">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="13"/>
       <c r="B255" s="13"/>
       <c r="E255" s="13"/>
@@ -5817,7 +5817,7 @@
       <c r="H255" s="13"/>
       <c r="I255" s="13"/>
     </row>
-    <row r="256" spans="1:9">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="13"/>
       <c r="B256" s="13"/>
       <c r="E256" s="13"/>
@@ -5826,7 +5826,7 @@
       <c r="H256" s="13"/>
       <c r="I256" s="13"/>
     </row>
-    <row r="257" spans="1:9">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" s="13"/>
       <c r="B257" s="13"/>
       <c r="E257" s="13"/>
@@ -5835,7 +5835,7 @@
       <c r="H257" s="13"/>
       <c r="I257" s="13"/>
     </row>
-    <row r="258" spans="1:9">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" s="13"/>
       <c r="B258" s="13"/>
       <c r="E258" s="13"/>
@@ -5844,7 +5844,7 @@
       <c r="H258" s="13"/>
       <c r="I258" s="13"/>
     </row>
-    <row r="259" spans="1:9">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" s="13"/>
       <c r="B259" s="13"/>
       <c r="E259" s="13"/>
@@ -5853,7 +5853,7 @@
       <c r="H259" s="13"/>
       <c r="I259" s="13"/>
     </row>
-    <row r="260" spans="1:9">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" s="13"/>
       <c r="B260" s="13"/>
       <c r="E260" s="13"/>
@@ -5862,7 +5862,7 @@
       <c r="H260" s="13"/>
       <c r="I260" s="13"/>
     </row>
-    <row r="261" spans="1:9">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" s="13"/>
       <c r="B261" s="13"/>
       <c r="E261" s="13"/>
@@ -5871,7 +5871,7 @@
       <c r="H261" s="13"/>
       <c r="I261" s="13"/>
     </row>
-    <row r="262" spans="1:9">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="13"/>
       <c r="B262" s="13"/>
       <c r="E262" s="13"/>
@@ -5880,7 +5880,7 @@
       <c r="H262" s="13"/>
       <c r="I262" s="13"/>
     </row>
-    <row r="263" spans="1:9">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="13"/>
       <c r="B263" s="13"/>
       <c r="E263" s="13"/>
@@ -5889,7 +5889,7 @@
       <c r="H263" s="13"/>
       <c r="I263" s="13"/>
     </row>
-    <row r="264" spans="1:9">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="13"/>
       <c r="B264" s="13"/>
       <c r="E264" s="13"/>
@@ -5898,7 +5898,7 @@
       <c r="H264" s="13"/>
       <c r="I264" s="13"/>
     </row>
-    <row r="265" spans="1:9">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" s="13"/>
       <c r="B265" s="13"/>
       <c r="E265" s="13"/>
@@ -5907,7 +5907,7 @@
       <c r="H265" s="13"/>
       <c r="I265" s="13"/>
     </row>
-    <row r="266" spans="1:9">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" s="13"/>
       <c r="B266" s="13"/>
       <c r="E266" s="13"/>
@@ -5916,7 +5916,7 @@
       <c r="H266" s="13"/>
       <c r="I266" s="13"/>
     </row>
-    <row r="267" spans="1:9">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" s="13"/>
       <c r="B267" s="13"/>
       <c r="E267" s="13"/>
@@ -5925,7 +5925,7 @@
       <c r="H267" s="13"/>
       <c r="I267" s="13"/>
     </row>
-    <row r="268" spans="1:9">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" s="13"/>
       <c r="B268" s="13"/>
       <c r="E268" s="13"/>
@@ -5934,7 +5934,7 @@
       <c r="H268" s="13"/>
       <c r="I268" s="13"/>
     </row>
-    <row r="269" spans="1:9" hidden="1">
+    <row r="269" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="13"/>
       <c r="B269" s="13"/>
       <c r="E269" s="13"/>
@@ -5943,7 +5943,7 @@
       <c r="H269" s="13"/>
       <c r="I269" s="13"/>
     </row>
-    <row r="270" spans="1:9" hidden="1">
+    <row r="270" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="13"/>
       <c r="B270" s="13"/>
       <c r="E270" s="13"/>
@@ -5952,7 +5952,7 @@
       <c r="H270" s="13"/>
       <c r="I270" s="13"/>
     </row>
-    <row r="271" spans="1:9" hidden="1">
+    <row r="271" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="13"/>
       <c r="B271" s="13"/>
       <c r="E271" s="13"/>
@@ -5961,7 +5961,7 @@
       <c r="H271" s="13"/>
       <c r="I271" s="13"/>
     </row>
-    <row r="272" spans="1:9" hidden="1">
+    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="13"/>
       <c r="B272" s="13"/>
       <c r="E272" s="13"/>
@@ -5970,7 +5970,7 @@
       <c r="H272" s="13"/>
       <c r="I272" s="13"/>
     </row>
-    <row r="273" spans="1:9" hidden="1">
+    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
       <c r="B273" s="13"/>
       <c r="E273" s="13"/>
@@ -5979,7 +5979,7 @@
       <c r="H273" s="13"/>
       <c r="I273" s="13"/>
     </row>
-    <row r="274" spans="1:9" hidden="1">
+    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="13"/>
       <c r="B274" s="13"/>
       <c r="E274" s="13"/>
@@ -5988,7 +5988,7 @@
       <c r="H274" s="13"/>
       <c r="I274" s="13"/>
     </row>
-    <row r="275" spans="1:9" hidden="1">
+    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="13"/>
       <c r="B275" s="13"/>
       <c r="E275" s="13"/>
@@ -5997,7 +5997,7 @@
       <c r="H275" s="13"/>
       <c r="I275" s="13"/>
     </row>
-    <row r="276" spans="1:9" hidden="1">
+    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="13"/>
       <c r="B276" s="13"/>
       <c r="E276" s="13"/>
@@ -6006,7 +6006,7 @@
       <c r="H276" s="13"/>
       <c r="I276" s="13"/>
     </row>
-    <row r="277" spans="1:9" hidden="1">
+    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="13"/>
       <c r="B277" s="13"/>
       <c r="E277" s="13"/>
@@ -6015,7 +6015,7 @@
       <c r="H277" s="13"/>
       <c r="I277" s="13"/>
     </row>
-    <row r="278" spans="1:9" hidden="1">
+    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="13"/>
       <c r="B278" s="13"/>
       <c r="E278" s="13"/>
@@ -6024,7 +6024,7 @@
       <c r="H278" s="13"/>
       <c r="I278" s="13"/>
     </row>
-    <row r="279" spans="1:9" hidden="1">
+    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="13"/>
       <c r="B279" s="13"/>
       <c r="E279" s="13"/>
@@ -6033,7 +6033,7 @@
       <c r="H279" s="13"/>
       <c r="I279" s="13"/>
     </row>
-    <row r="280" spans="1:9" hidden="1">
+    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="13"/>
       <c r="B280" s="13"/>
       <c r="E280" s="13"/>
@@ -6042,7 +6042,7 @@
       <c r="H280" s="13"/>
       <c r="I280" s="13"/>
     </row>
-    <row r="281" spans="1:9" hidden="1">
+    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="13"/>
       <c r="B281" s="13"/>
       <c r="E281" s="13"/>
@@ -6051,7 +6051,7 @@
       <c r="H281" s="13"/>
       <c r="I281" s="13"/>
     </row>
-    <row r="282" spans="1:9" hidden="1">
+    <row r="282" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="13"/>
       <c r="B282" s="13"/>
       <c r="E282" s="13"/>
@@ -6060,7 +6060,7 @@
       <c r="H282" s="13"/>
       <c r="I282" s="13"/>
     </row>
-    <row r="283" spans="1:9">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" s="13"/>
       <c r="B283" s="13"/>
       <c r="E283" s="13"/>
@@ -6069,7 +6069,7 @@
       <c r="H283" s="13"/>
       <c r="I283" s="13"/>
     </row>
-    <row r="284" spans="1:9">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" s="13"/>
       <c r="B284" s="13"/>
       <c r="E284" s="13"/>
@@ -6078,7 +6078,7 @@
       <c r="H284" s="13"/>
       <c r="I284" s="13"/>
     </row>
-    <row r="285" spans="1:9">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" s="13"/>
       <c r="B285" s="13"/>
       <c r="E285" s="13"/>
@@ -6087,7 +6087,7 @@
       <c r="H285" s="13"/>
       <c r="I285" s="13"/>
     </row>
-    <row r="286" spans="1:9">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" s="13"/>
       <c r="B286" s="13"/>
       <c r="E286" s="13"/>
@@ -6096,7 +6096,7 @@
       <c r="H286" s="13"/>
       <c r="I286" s="13"/>
     </row>
-    <row r="287" spans="1:9">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" s="13"/>
       <c r="B287" s="13"/>
       <c r="E287" s="13"/>
@@ -6105,7 +6105,7 @@
       <c r="H287" s="13"/>
       <c r="I287" s="13"/>
     </row>
-    <row r="288" spans="1:9">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" s="13"/>
       <c r="B288" s="13"/>
       <c r="E288" s="13"/>
@@ -6114,7 +6114,7 @@
       <c r="H288" s="13"/>
       <c r="I288" s="13"/>
     </row>
-    <row r="289" spans="1:9">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
       <c r="B289" s="13"/>
       <c r="E289" s="13"/>
@@ -6123,7 +6123,7 @@
       <c r="H289" s="13"/>
       <c r="I289" s="13"/>
     </row>
-    <row r="290" spans="1:9">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" s="13"/>
       <c r="B290" s="13"/>
       <c r="E290" s="13"/>
@@ -6132,7 +6132,7 @@
       <c r="H290" s="13"/>
       <c r="I290" s="13"/>
     </row>
-    <row r="291" spans="1:9">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" s="13"/>
       <c r="B291" s="13"/>
       <c r="E291" s="13"/>
@@ -6141,7 +6141,7 @@
       <c r="H291" s="13"/>
       <c r="I291" s="13"/>
     </row>
-    <row r="292" spans="1:9">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" s="13"/>
       <c r="B292" s="13"/>
       <c r="E292" s="13"/>
@@ -6150,7 +6150,7 @@
       <c r="H292" s="13"/>
       <c r="I292" s="13"/>
     </row>
-    <row r="293" spans="1:9">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" s="13"/>
       <c r="B293" s="13"/>
       <c r="E293" s="13"/>
@@ -6159,7 +6159,7 @@
       <c r="H293" s="13"/>
       <c r="I293" s="13"/>
     </row>
-    <row r="294" spans="1:9">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" s="13"/>
       <c r="B294" s="13"/>
       <c r="E294" s="13"/>
@@ -6168,7 +6168,7 @@
       <c r="H294" s="13"/>
       <c r="I294" s="13"/>
     </row>
-    <row r="295" spans="1:9">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" s="13"/>
       <c r="B295" s="13"/>
       <c r="E295" s="13"/>
@@ -6177,7 +6177,7 @@
       <c r="H295" s="13"/>
       <c r="I295" s="13"/>
     </row>
-    <row r="296" spans="1:9">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" s="13"/>
       <c r="B296" s="13"/>
       <c r="E296" s="13"/>
@@ -6186,7 +6186,7 @@
       <c r="H296" s="13"/>
       <c r="I296" s="13"/>
     </row>
-    <row r="297" spans="1:9">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" s="13"/>
       <c r="B297" s="13"/>
       <c r="E297" s="13"/>
@@ -6195,7 +6195,7 @@
       <c r="H297" s="13"/>
       <c r="I297" s="13"/>
     </row>
-    <row r="298" spans="1:9">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" s="13"/>
       <c r="B298" s="13"/>
       <c r="E298" s="13"/>
@@ -6204,7 +6204,7 @@
       <c r="H298" s="13"/>
       <c r="I298" s="13"/>
     </row>
-    <row r="299" spans="1:9">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" s="13"/>
       <c r="B299" s="13"/>
       <c r="E299" s="13"/>
@@ -6213,7 +6213,7 @@
       <c r="H299" s="13"/>
       <c r="I299" s="13"/>
     </row>
-    <row r="300" spans="1:9">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" s="13"/>
       <c r="B300" s="13"/>
       <c r="E300" s="13"/>
@@ -6222,7 +6222,7 @@
       <c r="H300" s="13"/>
       <c r="I300" s="13"/>
     </row>
-    <row r="301" spans="1:9">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" s="13"/>
       <c r="B301" s="13"/>
       <c r="E301" s="13"/>
@@ -6231,7 +6231,7 @@
       <c r="H301" s="13"/>
       <c r="I301" s="13"/>
     </row>
-    <row r="302" spans="1:9">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" s="13"/>
       <c r="B302" s="13"/>
       <c r="E302" s="13"/>
@@ -6240,7 +6240,7 @@
       <c r="H302" s="13"/>
       <c r="I302" s="13"/>
     </row>
-    <row r="303" spans="1:9">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" s="13"/>
       <c r="B303" s="13"/>
       <c r="E303" s="13"/>
@@ -6249,7 +6249,7 @@
       <c r="H303" s="13"/>
       <c r="I303" s="13"/>
     </row>
-    <row r="304" spans="1:9">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" s="13"/>
       <c r="B304" s="13"/>
       <c r="E304" s="13"/>
@@ -6258,7 +6258,7 @@
       <c r="H304" s="13"/>
       <c r="I304" s="13"/>
     </row>
-    <row r="305" spans="1:9">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" s="13"/>
       <c r="B305" s="13"/>
       <c r="E305" s="13"/>
@@ -6267,7 +6267,7 @@
       <c r="H305" s="13"/>
       <c r="I305" s="13"/>
     </row>
-    <row r="306" spans="1:9">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" s="13"/>
       <c r="B306" s="13"/>
       <c r="E306" s="13"/>
@@ -6276,7 +6276,7 @@
       <c r="H306" s="13"/>
       <c r="I306" s="13"/>
     </row>
-    <row r="307" spans="1:9">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" s="13"/>
       <c r="B307" s="13"/>
       <c r="E307" s="13"/>
@@ -6285,7 +6285,7 @@
       <c r="H307" s="13"/>
       <c r="I307" s="13"/>
     </row>
-    <row r="308" spans="1:9">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" s="13"/>
       <c r="B308" s="13"/>
       <c r="E308" s="13"/>
@@ -6294,7 +6294,7 @@
       <c r="H308" s="13"/>
       <c r="I308" s="13"/>
     </row>
-    <row r="309" spans="1:9">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" s="13"/>
       <c r="B309" s="13"/>
       <c r="E309" s="13"/>
@@ -6303,7 +6303,7 @@
       <c r="H309" s="13"/>
       <c r="I309" s="13"/>
     </row>
-    <row r="310" spans="1:9">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" s="13"/>
       <c r="B310" s="13"/>
       <c r="E310" s="13"/>
@@ -6312,7 +6312,7 @@
       <c r="H310" s="13"/>
       <c r="I310" s="13"/>
     </row>
-    <row r="311" spans="1:9">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" s="13"/>
       <c r="B311" s="13"/>
       <c r="E311" s="13"/>
@@ -6321,7 +6321,7 @@
       <c r="H311" s="13"/>
       <c r="I311" s="13"/>
     </row>
-    <row r="312" spans="1:9">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" s="13"/>
       <c r="B312" s="13"/>
       <c r="E312" s="13"/>
@@ -6330,7 +6330,7 @@
       <c r="H312" s="13"/>
       <c r="I312" s="13"/>
     </row>
-    <row r="313" spans="1:9">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" s="13"/>
       <c r="B313" s="13"/>
       <c r="E313" s="13"/>
@@ -6339,7 +6339,7 @@
       <c r="H313" s="13"/>
       <c r="I313" s="13"/>
     </row>
-    <row r="314" spans="1:9">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" s="13"/>
       <c r="B314" s="13"/>
       <c r="E314" s="13"/>
@@ -6348,7 +6348,7 @@
       <c r="H314" s="13"/>
       <c r="I314" s="13"/>
     </row>
-    <row r="315" spans="1:9">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" s="13"/>
       <c r="B315" s="13"/>
       <c r="E315" s="13"/>
@@ -6357,7 +6357,7 @@
       <c r="H315" s="13"/>
       <c r="I315" s="13"/>
     </row>
-    <row r="316" spans="1:9">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" s="13"/>
       <c r="B316" s="13"/>
       <c r="E316" s="13"/>
@@ -6366,7 +6366,7 @@
       <c r="H316" s="13"/>
       <c r="I316" s="13"/>
     </row>
-    <row r="317" spans="1:9">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" s="13"/>
       <c r="B317" s="13"/>
       <c r="E317" s="13"/>
@@ -6375,7 +6375,7 @@
       <c r="H317" s="13"/>
       <c r="I317" s="13"/>
     </row>
-    <row r="318" spans="1:9">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" s="13"/>
       <c r="B318" s="13"/>
       <c r="E318" s="13"/>
@@ -6384,7 +6384,7 @@
       <c r="H318" s="13"/>
       <c r="I318" s="13"/>
     </row>
-    <row r="319" spans="1:9">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A319" s="13"/>
       <c r="B319" s="13"/>
       <c r="E319" s="13"/>
@@ -6393,7 +6393,7 @@
       <c r="H319" s="13"/>
       <c r="I319" s="13"/>
     </row>
-    <row r="320" spans="1:9">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A320" s="13"/>
       <c r="B320" s="13"/>
       <c r="E320" s="13"/>
@@ -6402,7 +6402,7 @@
       <c r="H320" s="13"/>
       <c r="I320" s="13"/>
     </row>
-    <row r="321" spans="1:9">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A321" s="13"/>
       <c r="B321" s="13"/>
       <c r="E321" s="13"/>
@@ -6411,7 +6411,7 @@
       <c r="H321" s="13"/>
       <c r="I321" s="13"/>
     </row>
-    <row r="322" spans="1:9">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A322" s="13"/>
       <c r="B322" s="13"/>
       <c r="E322" s="13"/>
@@ -6420,7 +6420,7 @@
       <c r="H322" s="13"/>
       <c r="I322" s="13"/>
     </row>
-    <row r="323" spans="1:9">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A323" s="13"/>
       <c r="B323" s="13"/>
       <c r="E323" s="13"/>
@@ -6429,7 +6429,7 @@
       <c r="H323" s="13"/>
       <c r="I323" s="13"/>
     </row>
-    <row r="324" spans="1:9">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A324" s="13"/>
       <c r="B324" s="13"/>
       <c r="E324" s="13"/>
@@ -6438,7 +6438,7 @@
       <c r="H324" s="13"/>
       <c r="I324" s="13"/>
     </row>
-    <row r="325" spans="1:9">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A325" s="13"/>
       <c r="B325" s="13"/>
       <c r="E325" s="13"/>
@@ -6447,7 +6447,7 @@
       <c r="H325" s="13"/>
       <c r="I325" s="13"/>
     </row>
-    <row r="326" spans="1:9">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A326" s="13"/>
       <c r="B326" s="13"/>
       <c r="E326" s="13"/>
@@ -6456,7 +6456,7 @@
       <c r="H326" s="13"/>
       <c r="I326" s="13"/>
     </row>
-    <row r="327" spans="1:9">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A327" s="13"/>
       <c r="B327" s="13"/>
       <c r="E327" s="13"/>
@@ -6465,7 +6465,7 @@
       <c r="H327" s="13"/>
       <c r="I327" s="13"/>
     </row>
-    <row r="328" spans="1:9">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A328" s="13"/>
       <c r="B328" s="13"/>
       <c r="E328" s="13"/>
@@ -6474,7 +6474,7 @@
       <c r="H328" s="13"/>
       <c r="I328" s="13"/>
     </row>
-    <row r="329" spans="1:9">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A329" s="13"/>
       <c r="B329" s="13"/>
       <c r="E329" s="13"/>
@@ -6483,7 +6483,7 @@
       <c r="H329" s="13"/>
       <c r="I329" s="13"/>
     </row>
-    <row r="330" spans="1:9">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A330" s="13"/>
       <c r="B330" s="13"/>
       <c r="E330" s="13"/>
@@ -6492,7 +6492,7 @@
       <c r="H330" s="13"/>
       <c r="I330" s="13"/>
     </row>
-    <row r="331" spans="1:9">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A331" s="13"/>
       <c r="B331" s="13"/>
       <c r="E331" s="13"/>
@@ -6501,7 +6501,7 @@
       <c r="H331" s="13"/>
       <c r="I331" s="13"/>
     </row>
-    <row r="332" spans="1:9">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A332" s="13"/>
       <c r="B332" s="13"/>
       <c r="E332" s="13"/>
@@ -6510,7 +6510,7 @@
       <c r="H332" s="13"/>
       <c r="I332" s="13"/>
     </row>
-    <row r="333" spans="1:9">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A333" s="13"/>
       <c r="B333" s="13"/>
       <c r="E333" s="13"/>
@@ -6519,7 +6519,7 @@
       <c r="H333" s="13"/>
       <c r="I333" s="13"/>
     </row>
-    <row r="334" spans="1:9">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A334" s="13"/>
       <c r="B334" s="13"/>
       <c r="E334" s="13"/>
@@ -6528,7 +6528,7 @@
       <c r="H334" s="13"/>
       <c r="I334" s="13"/>
     </row>
-    <row r="335" spans="1:9">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A335" s="13"/>
       <c r="B335" s="13"/>
       <c r="E335" s="13"/>
@@ -6537,7 +6537,7 @@
       <c r="H335" s="13"/>
       <c r="I335" s="13"/>
     </row>
-    <row r="336" spans="1:9">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A336" s="13"/>
       <c r="B336" s="13"/>
       <c r="E336" s="13"/>
@@ -6546,7 +6546,7 @@
       <c r="H336" s="13"/>
       <c r="I336" s="13"/>
     </row>
-    <row r="337" spans="1:9">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" s="13"/>
       <c r="B337" s="13"/>
       <c r="E337" s="13"/>
@@ -6555,7 +6555,7 @@
       <c r="H337" s="13"/>
       <c r="I337" s="13"/>
     </row>
-    <row r="338" spans="1:9">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" s="13"/>
       <c r="B338" s="13"/>
       <c r="E338" s="13"/>
@@ -6564,7 +6564,7 @@
       <c r="H338" s="13"/>
       <c r="I338" s="13"/>
     </row>
-    <row r="339" spans="1:9">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A339" s="13"/>
       <c r="B339" s="13"/>
       <c r="E339" s="13"/>
@@ -6573,7 +6573,7 @@
       <c r="H339" s="13"/>
       <c r="I339" s="13"/>
     </row>
-    <row r="340" spans="1:9">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" s="13"/>
       <c r="B340" s="13"/>
       <c r="E340" s="13"/>
@@ -6582,7 +6582,7 @@
       <c r="H340" s="13"/>
       <c r="I340" s="13"/>
     </row>
-    <row r="341" spans="1:9">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A341" s="13"/>
       <c r="B341" s="13"/>
       <c r="E341" s="13"/>
@@ -6591,7 +6591,7 @@
       <c r="H341" s="13"/>
       <c r="I341" s="13"/>
     </row>
-    <row r="342" spans="1:9">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A342" s="13"/>
       <c r="B342" s="13"/>
       <c r="E342" s="13"/>
@@ -6600,7 +6600,7 @@
       <c r="H342" s="13"/>
       <c r="I342" s="13"/>
     </row>
-    <row r="343" spans="1:9">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A343" s="13"/>
       <c r="B343" s="13"/>
       <c r="E343" s="13"/>
@@ -6609,7 +6609,7 @@
       <c r="H343" s="13"/>
       <c r="I343" s="13"/>
     </row>
-    <row r="344" spans="1:9">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A344" s="13"/>
       <c r="B344" s="13"/>
       <c r="E344" s="13"/>
@@ -6618,7 +6618,7 @@
       <c r="H344" s="13"/>
       <c r="I344" s="13"/>
     </row>
-    <row r="345" spans="1:9">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A345" s="13"/>
       <c r="B345" s="13"/>
       <c r="E345" s="13"/>
@@ -6627,7 +6627,7 @@
       <c r="H345" s="13"/>
       <c r="I345" s="13"/>
     </row>
-    <row r="346" spans="1:9">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A346" s="13"/>
       <c r="B346" s="13"/>
       <c r="E346" s="13"/>
@@ -6636,7 +6636,7 @@
       <c r="H346" s="13"/>
       <c r="I346" s="13"/>
     </row>
-    <row r="347" spans="1:9">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A347" s="13"/>
       <c r="B347" s="13"/>
       <c r="E347" s="13"/>
@@ -6645,7 +6645,7 @@
       <c r="H347" s="13"/>
       <c r="I347" s="13"/>
     </row>
-    <row r="348" spans="1:9">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A348" s="13"/>
       <c r="B348" s="13"/>
       <c r="E348" s="13"/>
@@ -6654,7 +6654,7 @@
       <c r="H348" s="13"/>
       <c r="I348" s="13"/>
     </row>
-    <row r="349" spans="1:9">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A349" s="13"/>
       <c r="B349" s="13"/>
       <c r="E349" s="13"/>
@@ -6663,7 +6663,7 @@
       <c r="H349" s="13"/>
       <c r="I349" s="13"/>
     </row>
-    <row r="350" spans="1:9">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A350" s="13"/>
       <c r="B350" s="13"/>
       <c r="E350" s="13"/>
@@ -6672,7 +6672,7 @@
       <c r="H350" s="13"/>
       <c r="I350" s="13"/>
     </row>
-    <row r="351" spans="1:9">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A351" s="13"/>
       <c r="B351" s="13"/>
       <c r="E351" s="13"/>
@@ -6681,7 +6681,7 @@
       <c r="H351" s="13"/>
       <c r="I351" s="13"/>
     </row>
-    <row r="352" spans="1:9">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A352" s="13"/>
       <c r="B352" s="13"/>
       <c r="E352" s="13"/>
@@ -6690,7 +6690,7 @@
       <c r="H352" s="13"/>
       <c r="I352" s="13"/>
     </row>
-    <row r="353" spans="1:9">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A353" s="13"/>
       <c r="B353" s="13"/>
       <c r="E353" s="13"/>
@@ -6699,7 +6699,7 @@
       <c r="H353" s="13"/>
       <c r="I353" s="13"/>
     </row>
-    <row r="354" spans="1:9">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A354" s="13"/>
       <c r="B354" s="13"/>
       <c r="E354" s="13"/>
@@ -6708,7 +6708,7 @@
       <c r="H354" s="13"/>
       <c r="I354" s="13"/>
     </row>
-    <row r="355" spans="1:9">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A355" s="13"/>
       <c r="B355" s="13"/>
       <c r="E355" s="13"/>
@@ -6717,7 +6717,7 @@
       <c r="H355" s="13"/>
       <c r="I355" s="13"/>
     </row>
-    <row r="356" spans="1:9">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A356" s="13"/>
       <c r="B356" s="13"/>
       <c r="E356" s="13"/>
@@ -6726,7 +6726,7 @@
       <c r="H356" s="13"/>
       <c r="I356" s="13"/>
     </row>
-    <row r="357" spans="1:9">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A357" s="13"/>
       <c r="B357" s="13"/>
       <c r="E357" s="13"/>
@@ -6735,7 +6735,7 @@
       <c r="H357" s="13"/>
       <c r="I357" s="13"/>
     </row>
-    <row r="358" spans="1:9">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A358" s="13"/>
       <c r="B358" s="13"/>
       <c r="E358" s="13"/>
@@ -6744,7 +6744,7 @@
       <c r="H358" s="13"/>
       <c r="I358" s="13"/>
     </row>
-    <row r="359" spans="1:9">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A359" s="13"/>
       <c r="B359" s="13"/>
       <c r="E359" s="13"/>
@@ -6753,7 +6753,7 @@
       <c r="H359" s="13"/>
       <c r="I359" s="13"/>
     </row>
-    <row r="360" spans="1:9">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A360" s="13"/>
       <c r="B360" s="13"/>
       <c r="E360" s="13"/>
@@ -6762,7 +6762,7 @@
       <c r="H360" s="13"/>
       <c r="I360" s="13"/>
     </row>
-    <row r="361" spans="1:9">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A361" s="13"/>
       <c r="B361" s="13"/>
       <c r="E361" s="13"/>
@@ -6771,7 +6771,7 @@
       <c r="H361" s="13"/>
       <c r="I361" s="13"/>
     </row>
-    <row r="362" spans="1:9">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A362" s="13"/>
       <c r="B362" s="13"/>
       <c r="E362" s="13"/>
@@ -6780,7 +6780,7 @@
       <c r="H362" s="13"/>
       <c r="I362" s="13"/>
     </row>
-    <row r="363" spans="1:9">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A363" s="13"/>
       <c r="B363" s="13"/>
       <c r="E363" s="13"/>
@@ -6789,7 +6789,7 @@
       <c r="H363" s="13"/>
       <c r="I363" s="13"/>
     </row>
-    <row r="364" spans="1:9">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A364" s="13"/>
       <c r="B364" s="13"/>
       <c r="E364" s="13"/>
@@ -6798,7 +6798,7 @@
       <c r="H364" s="13"/>
       <c r="I364" s="13"/>
     </row>
-    <row r="365" spans="1:9">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A365" s="13"/>
       <c r="B365" s="13"/>
       <c r="E365" s="13"/>
@@ -6807,7 +6807,7 @@
       <c r="H365" s="13"/>
       <c r="I365" s="13"/>
     </row>
-    <row r="366" spans="1:9">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A366" s="13"/>
       <c r="B366" s="13"/>
       <c r="E366" s="13"/>
@@ -6816,7 +6816,7 @@
       <c r="H366" s="13"/>
       <c r="I366" s="13"/>
     </row>
-    <row r="367" spans="1:9">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A367" s="13"/>
       <c r="B367" s="13"/>
       <c r="E367" s="13"/>
@@ -6825,7 +6825,7 @@
       <c r="H367" s="13"/>
       <c r="I367" s="13"/>
     </row>
-    <row r="368" spans="1:9">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A368" s="13"/>
       <c r="B368" s="13"/>
       <c r="E368" s="13"/>
@@ -6834,7 +6834,7 @@
       <c r="H368" s="13"/>
       <c r="I368" s="13"/>
     </row>
-    <row r="369" spans="1:9">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A369" s="13"/>
       <c r="B369" s="13"/>
       <c r="E369" s="13"/>
@@ -6843,7 +6843,7 @@
       <c r="H369" s="13"/>
       <c r="I369" s="13"/>
     </row>
-    <row r="370" spans="1:9">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A370" s="13"/>
       <c r="B370" s="13"/>
       <c r="E370" s="13"/>
@@ -6852,7 +6852,7 @@
       <c r="H370" s="13"/>
       <c r="I370" s="13"/>
     </row>
-    <row r="371" spans="1:9">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A371" s="13"/>
       <c r="B371" s="13"/>
       <c r="E371" s="13"/>
@@ -6861,7 +6861,7 @@
       <c r="H371" s="13"/>
       <c r="I371" s="13"/>
     </row>
-    <row r="372" spans="1:9">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A372" s="13"/>
       <c r="B372" s="13"/>
       <c r="E372" s="13"/>
@@ -6870,7 +6870,7 @@
       <c r="H372" s="13"/>
       <c r="I372" s="13"/>
     </row>
-    <row r="373" spans="1:9">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A373" s="13"/>
       <c r="B373" s="13"/>
       <c r="E373" s="13"/>
@@ -6879,7 +6879,7 @@
       <c r="H373" s="13"/>
       <c r="I373" s="13"/>
     </row>
-    <row r="374" spans="1:9">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A374" s="13"/>
       <c r="B374" s="13"/>
       <c r="E374" s="13"/>
@@ -6888,7 +6888,7 @@
       <c r="H374" s="13"/>
       <c r="I374" s="13"/>
     </row>
-    <row r="375" spans="1:9">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A375" s="13"/>
       <c r="B375" s="13"/>
       <c r="E375" s="13"/>
@@ -6897,7 +6897,7 @@
       <c r="H375" s="13"/>
       <c r="I375" s="13"/>
     </row>
-    <row r="376" spans="1:9">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A376" s="13"/>
       <c r="B376" s="13"/>
       <c r="E376" s="13"/>
@@ -6906,7 +6906,7 @@
       <c r="H376" s="13"/>
       <c r="I376" s="13"/>
     </row>
-    <row r="377" spans="1:9">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A377" s="13"/>
       <c r="B377" s="13"/>
       <c r="E377" s="13"/>
@@ -6915,7 +6915,7 @@
       <c r="H377" s="13"/>
       <c r="I377" s="13"/>
     </row>
-    <row r="378" spans="1:9">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A378" s="13"/>
       <c r="B378" s="13"/>
       <c r="E378" s="13"/>
@@ -6924,7 +6924,7 @@
       <c r="H378" s="13"/>
       <c r="I378" s="13"/>
     </row>
-    <row r="379" spans="1:9">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A379" s="13"/>
       <c r="B379" s="13"/>
       <c r="E379" s="13"/>
@@ -6933,7 +6933,7 @@
       <c r="H379" s="13"/>
       <c r="I379" s="13"/>
     </row>
-    <row r="380" spans="1:9">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A380" s="13"/>
       <c r="B380" s="13"/>
       <c r="E380" s="13"/>

</xml_diff>